<commit_message>
continue working on frontend ui and backend API
</commit_message>
<xml_diff>
--- a/NewCDSDataFromClient/CDSDefinitions.xlsx
+++ b/NewCDSDataFromClient/CDSDefinitions.xlsx
@@ -5,16 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\rhit_IRPA_2023\NewCDSDataFromClient\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zhengy6\Desktop\irpa_db\rhit_IRPA_2023\NewCDSDataFromClient\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70211441-04CA-40B9-8FA0-C6D0B18F3C4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CA7444-8E29-410A-8F00-072DD0FC75C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definition_General" sheetId="1" r:id="rId1"/>
-    <sheet name="Defintion_General 2" sheetId="3" r:id="rId2"/>
+    <sheet name="Definition_General 2" sheetId="3" r:id="rId2"/>
     <sheet name="Definition_Financial Aid" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="126">
   <si>
     <t>Question</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>What is the definition for work study and employment?</t>
+  </si>
+  <si>
+    <t>test</t>
   </si>
 </sst>
 </file>
@@ -736,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -758,275 +761,440 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1039,8 +1207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C4990CF-594D-44E7-8ED2-EB98FC4D9840}">
   <dimension ref="A1:B58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="F51" sqref="F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1061,285 +1229,456 @@
       <c r="A2" s="3" t="s">
         <v>57</v>
       </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>58</v>
       </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="4" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>59</v>
       </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>60</v>
       </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>62</v>
       </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>64</v>
       </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>65</v>
       </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>66</v>
       </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>67</v>
       </c>
+      <c r="B12" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>68</v>
       </c>
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="14" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>69</v>
       </c>
+      <c r="B14" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>70</v>
       </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B17" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B20" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B24" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B26" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B29" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B30" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B31" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B32" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A34" s="3" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B34" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="3" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="3" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="3" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="42" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B41" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A42" s="3" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B42" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="3" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B43" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="3" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B44" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="3" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="46" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B45" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A46" s="3" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B46" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="3" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B47" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="3" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B48" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="3" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B49" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="3" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B50" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B51" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="3" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B52" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="3" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B53" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="3" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B55" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="B56" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="58" spans="1:1" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="B57" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A58" s="3" t="s">
         <v>113</v>
+      </c>
+      <c r="B58" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1351,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756BDE7E-EB4E-4DC0-95D6-8C6E695703B2}">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1373,55 +1712,88 @@
       <c r="A2" s="3" t="s">
         <v>114</v>
       </c>
+      <c r="B2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>115</v>
       </c>
+      <c r="B3" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>116</v>
       </c>
+      <c r="B4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>117</v>
       </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>118</v>
       </c>
+      <c r="B6" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>119</v>
       </c>
+      <c r="B7" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>120</v>
       </c>
+      <c r="B8" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>121</v>
       </c>
+      <c r="B9" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="10" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>122</v>
       </c>
+      <c r="B10" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>123</v>
       </c>
+      <c r="B11" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="12" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>124</v>
+      </c>
+      <c r="B12" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>